<commit_message>
fix kaiki and processing
</commit_message>
<xml_diff>
--- a/AkioAI/maxinfo/中山芝1200.xlsx
+++ b/AkioAI/maxinfo/中山芝1200.xlsx
@@ -15,7 +15,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1</t>
+  </si>
   <si>
     <t>max</t>
   </si>
@@ -405,23 +411,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.3541453925452973</v>
       </c>
     </row>
   </sheetData>
@@ -431,116 +449,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>0</v>
       </c>
     </row>

</xml_diff>